<commit_message>
fixed number of examples to correct value
</commit_message>
<xml_diff>
--- a/data/working/diagnostic_plots.xlsx
+++ b/data/working/diagnostic_plots.xlsx
@@ -114,12 +114,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -147,6 +153,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,11 +281,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41415424"/>
-        <c:axId val="41416960"/>
+        <c:axId val="52961280"/>
+        <c:axId val="52962816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41415424"/>
+        <c:axId val="52961280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -296,7 +304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41416960"/>
+        <c:crossAx val="52962816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -304,7 +312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41416960"/>
+        <c:axId val="52962816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +323,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41415424"/>
+        <c:crossAx val="52961280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -834,11 +842,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41449728"/>
-        <c:axId val="41455616"/>
+        <c:axId val="82318848"/>
+        <c:axId val="82320384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41449728"/>
+        <c:axId val="82318848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -862,13 +870,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41455616"/>
+        <c:crossAx val="82320384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41455616"/>
+        <c:axId val="82320384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -896,7 +904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41449728"/>
+        <c:crossAx val="82318848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -943,7 +951,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1184,11 +1191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41762816"/>
-        <c:axId val="41764736"/>
+        <c:axId val="82516992"/>
+        <c:axId val="82519168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41762816"/>
+        <c:axId val="82516992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1210,13 +1217,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41764736"/>
+        <c:crossAx val="82519168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41764736"/>
+        <c:axId val="82519168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1245,7 +1252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41762816"/>
+        <c:crossAx val="82516992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1361,10 +1368,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>diagnostics!$K$4:$K$17</c:f>
+              <c:f>diagnostics!$K$4:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -1402,20 +1409,17 @@
                   <c:v>110000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>132173</c:v>
+                  <c:v>115705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>diagnostics!$N$4:$N$17</c:f>
+              <c:f>diagnostics!$N$4:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1453,9 +1457,6 @@
                   <c:v>2.8159999999999963E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.8900000000000037E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>2.8900000000000037E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1496,10 +1497,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>diagnostics!$K$4:$K$17</c:f>
+              <c:f>diagnostics!$K$4:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -1537,20 +1538,17 @@
                   <c:v>110000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>132173</c:v>
+                  <c:v>115705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>diagnostics!$O$4:$O$17</c:f>
+              <c:f>diagnostics!$O$4:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.11600999999999995</c:v>
                 </c:pt>
@@ -1588,9 +1586,6 @@
                   <c:v>4.5569999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5290000000000052E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>4.5290000000000052E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1606,14 +1601,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41789696"/>
-        <c:axId val="41792256"/>
+        <c:axId val="82613760"/>
+        <c:axId val="82632704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41789696"/>
+        <c:axId val="82613760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="140000"/>
+          <c:max val="120000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1632,7 +1627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41792256"/>
+        <c:crossAx val="82632704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20000"/>
@@ -1641,7 +1636,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41792256"/>
+        <c:axId val="82632704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1668,7 +1663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41789696"/>
+        <c:crossAx val="82613760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2497,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3050,7 +3045,8 @@
         <v>6.336E-2</v>
       </c>
       <c r="K16" s="4">
-        <v>120000</v>
+        <f>165633-49928</f>
+        <v>115705</v>
       </c>
       <c r="L16" s="4">
         <v>0.97109999999999996</v>
@@ -3074,20 +3070,20 @@
       <c r="B17" s="6">
         <v>6.1080000000000002E-2</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="9">
         <v>132173</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="9">
         <v>0.97109999999999996</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="9">
         <v>0.95470999999999995</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="10">
         <f t="shared" si="2"/>
         <v>2.8900000000000037E-2</v>
       </c>
-      <c r="O17" s="8">
+      <c r="O17" s="10">
         <f t="shared" si="3"/>
         <v>4.5290000000000052E-2</v>
       </c>
@@ -3178,6 +3174,10 @@
       </c>
       <c r="B28" s="6">
         <v>4.4569999999999999E-2</v>
+      </c>
+      <c r="L28" s="4">
+        <f>165633-49928</f>
+        <v>115705</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>